<commit_message>
finish laporan lipa 5
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_2.xlsx
+++ b/hasil/2023_01_lipa_2.xlsx
@@ -293,10 +293,15 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -307,15 +312,10 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <left style="thin">
+      <top style="thin">
         <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="double">
+      </top>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -360,16 +360,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
@@ -380,20 +392,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
   </cellXfs>
@@ -718,52 +718,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:16" customHeight="1" ht="15.6">
       <c r="A4" s="3"/>
@@ -782,13 +782,13 @@
       </c>
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -801,52 +801,52 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:16" customHeight="1" ht="31.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="13"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:16" customHeight="1" ht="28.8">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:16" customHeight="1" ht="16.2">
@@ -2377,12 +2377,6 @@
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="E6:E7"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
@@ -2393,10 +2387,16 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="L5:L7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="1.46" right="0.19685039370079" top="0.43307086614173" bottom="0.43307086614173" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="5" orientation="landscape" scale="95" fitToHeight="1" fitToWidth="1"/>
+  <pageMargins left="0.62992125984252" right="0.43307086614173" top="0.43307086614173" bottom="0.43307086614173" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="272" orientation="landscape" scale="95" fitToHeight="1" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
finish create simpan/insert lipa 14
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_2.xlsx
+++ b/hasil/2023_01_lipa_2.xlsx
@@ -151,7 +151,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 10 Maret 2023</t>
+    <t>Ternate , 13 Maret 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -360,22 +360,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -388,12 +372,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
   </cellXfs>
@@ -718,52 +718,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:16" customHeight="1" ht="15.6">
       <c r="A4" s="3"/>
@@ -782,72 +782,72 @@
       </c>
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="14" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:16" customHeight="1" ht="31.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:16" customHeight="1" ht="28.8">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="16"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:16" customHeight="1" ht="16.2">
       <c r="A8" s="8">
@@ -2377,6 +2377,12 @@
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
@@ -2387,16 +2393,10 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="L5:L7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.62992125984252" right="0.43307086614173" top="0.43307086614173" bottom="0.43307086614173" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="272" orientation="landscape" scale="95" fitToHeight="1" fitToWidth="1"/>
+  <pageMargins left="0.59055118110236" right="0.43307086614173" top="0.43307086614173" bottom="0.43307086614173" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="14" orientation="landscape" scale="93" fitToHeight="1" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>